<commit_message>
Task #24: added data generation, storing and using from Excel file
</commit_message>
<xml_diff>
--- a/data/groups.xlsx
+++ b/data/groups.xlsx
@@ -26,19 +26,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t xml:space="preserve">NameKq&lt;le </t>
-  </si>
-  <si>
-    <t>NamesQN&amp;GL0a=</t>
-  </si>
-  <si>
-    <t>NameE-Z*auR5`</t>
-  </si>
-  <si>
-    <t>NameBDMd</t>
-  </si>
-  <si>
-    <t>NameG</t>
+    <t>Group F3E qsQDUv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group Lf7G 8 c  </t>
+  </si>
+  <si>
+    <t>Group b fF TO Va</t>
+  </si>
+  <si>
+    <t>Group FRS zalFlX</t>
+  </si>
+  <si>
+    <t>Group 8fUEBFhb0P</t>
   </si>
 </sst>
 </file>

</xml_diff>